<commit_message>
funcionalidades para atualizar informativo
</commit_message>
<xml_diff>
--- a/ligaroletarussa2021.xlsx
+++ b/ligaroletarussa2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristiano\Documents\LigaRoletaRussa2021\automacao_ligaroletarussa2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD2C790-D04E-4EA3-984C-08DABC933EF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF40114-3C3D-43CE-A49B-EAD409138D0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" tabRatio="598" xr2:uid="{89EF3BF4-4FB7-4847-9095-9B3A50FD985B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" tabRatio="598" activeTab="1" xr2:uid="{89EF3BF4-4FB7-4847-9095-9B3A50FD985B}"/>
   </bookViews>
   <sheets>
     <sheet name="Informativo" sheetId="1" r:id="rId1"/>
@@ -625,7 +625,64 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -634,64 +691,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1015,7 +1015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46AED9EE-0796-4882-8353-14CDACCF39CB}">
   <dimension ref="B2:BB36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AM13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="AM1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="BB34" sqref="BB34"/>
     </sheetView>
   </sheetViews>
@@ -1069,70 +1069,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:54" s="18" customFormat="1" ht="30" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="G2" s="23" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="G2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="L2" s="23" t="s">
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="L2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="Q2" s="23" t="s">
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="Q2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="W2" s="30" t="s">
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="W2" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AB2" s="23" t="s">
+      <c r="X2" s="42"/>
+      <c r="Y2" s="42"/>
+      <c r="Z2" s="42"/>
+      <c r="AB2" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
-      <c r="AH2" s="23" t="s">
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AH2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="AI2" s="23"/>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="23"/>
-      <c r="AM2" s="23" t="s">
+      <c r="AI2" s="34"/>
+      <c r="AJ2" s="34"/>
+      <c r="AK2" s="34"/>
+      <c r="AM2" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="AN2" s="23"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="23"/>
-      <c r="AR2" s="23" t="s">
+      <c r="AN2" s="34"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
+      <c r="AR2" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="AS2" s="23"/>
-      <c r="AT2" s="23"/>
-      <c r="AU2" s="23"/>
-      <c r="AV2" s="23"/>
-      <c r="AW2" s="23"/>
-      <c r="AY2" s="23" t="s">
+      <c r="AS2" s="34"/>
+      <c r="AT2" s="34"/>
+      <c r="AU2" s="34"/>
+      <c r="AV2" s="34"/>
+      <c r="AW2" s="34"/>
+      <c r="AY2" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="AZ2" s="23"/>
-      <c r="BA2" s="23"/>
-      <c r="BB2" s="23"/>
+      <c r="AZ2" s="34"/>
+      <c r="BA2" s="34"/>
+      <c r="BB2" s="34"/>
     </row>
     <row r="3" spans="2:54" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -1189,7 +1189,7 @@
         <v>22</v>
       </c>
       <c r="AB3" s="5"/>
-      <c r="AC3" s="32"/>
+      <c r="AC3" s="23"/>
       <c r="AD3" s="16" t="s">
         <v>12</v>
       </c>
@@ -1246,7 +1246,7 @@
         <f>LigaPrincipal!G3</f>
         <v>0</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="24">
         <v>150</v>
       </c>
       <c r="G4" s="13" t="s">
@@ -1260,7 +1260,7 @@
         <f>LigaPrincipal!G9</f>
         <v>0</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="24">
         <v>150</v>
       </c>
       <c r="L4" s="13" t="s">
@@ -1274,7 +1274,7 @@
         <f>LigaPrincipal!G15</f>
         <v>0</v>
       </c>
-      <c r="O4" s="33">
+      <c r="O4" s="24">
         <v>150</v>
       </c>
       <c r="Q4" s="13" t="s">
@@ -1292,7 +1292,7 @@
         <f>LigaPrincipal!H21</f>
         <v>0</v>
       </c>
-      <c r="U4" s="33">
+      <c r="U4" s="24">
         <v>150</v>
       </c>
       <c r="W4" s="13" t="s">
@@ -1306,10 +1306,10 @@
         <f>LigaPrincipal!C3</f>
         <v>0</v>
       </c>
-      <c r="Z4" s="36">
+      <c r="Z4" s="27">
         <v>1600</v>
       </c>
-      <c r="AB4" s="24" t="s">
+      <c r="AB4" s="43" t="s">
         <v>29</v>
       </c>
       <c r="AC4" s="13" t="s">
@@ -1323,27 +1323,27 @@
         <f>LigaPrincipal!M3</f>
         <v>0</v>
       </c>
-      <c r="AF4" s="36">
+      <c r="AF4" s="27">
         <v>100</v>
       </c>
-      <c r="AH4" s="26">
+      <c r="AH4" s="38">
         <v>1</v>
       </c>
       <c r="AI4" s="13" t="s">
         <v>24</v>
       </c>
       <c r="AJ4" s="19"/>
-      <c r="AK4" s="36">
+      <c r="AK4" s="27">
         <v>150</v>
       </c>
-      <c r="AM4" s="26">
+      <c r="AM4" s="38">
         <v>1</v>
       </c>
       <c r="AN4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="AO4" s="19"/>
-      <c r="AP4" s="36">
+      <c r="AP4" s="27">
         <v>150</v>
       </c>
       <c r="AR4" s="13" t="s">
@@ -1368,14 +1368,14 @@
         <f>LigaEliminatória!C28</f>
         <v>0</v>
       </c>
-      <c r="AY4" s="26">
+      <c r="AY4" s="38">
         <v>1</v>
       </c>
       <c r="AZ4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="BA4" s="19"/>
-      <c r="BB4" s="36">
+      <c r="BB4" s="27">
         <v>300</v>
       </c>
     </row>
@@ -1391,7 +1391,7 @@
         <f>LigaPrincipal!G4</f>
         <v>0</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="25">
         <v>100</v>
       </c>
       <c r="G5" s="14" t="s">
@@ -1405,7 +1405,7 @@
         <f>LigaPrincipal!G10</f>
         <v>0</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="25">
         <v>100</v>
       </c>
       <c r="L5" s="14" t="s">
@@ -1419,7 +1419,7 @@
         <f>LigaPrincipal!G16</f>
         <v>0</v>
       </c>
-      <c r="O5" s="34">
+      <c r="O5" s="25">
         <v>100</v>
       </c>
       <c r="Q5" s="14" t="s">
@@ -1437,7 +1437,7 @@
         <f>LigaPrincipal!H22</f>
         <v>0</v>
       </c>
-      <c r="U5" s="34">
+      <c r="U5" s="25">
         <v>100</v>
       </c>
       <c r="W5" s="14" t="s">
@@ -1451,10 +1451,10 @@
         <f>LigaPrincipal!C4</f>
         <v>1</v>
       </c>
-      <c r="Z5" s="34">
+      <c r="Z5" s="25">
         <v>800</v>
       </c>
-      <c r="AB5" s="25"/>
+      <c r="AB5" s="44"/>
       <c r="AC5" s="15" t="s">
         <v>10</v>
       </c>
@@ -1466,23 +1466,23 @@
         <f>LigaPrincipal!M4</f>
         <v>0</v>
       </c>
-      <c r="AF5" s="35">
+      <c r="AF5" s="26">
         <v>50</v>
       </c>
-      <c r="AH5" s="27"/>
+      <c r="AH5" s="39"/>
       <c r="AI5" s="14" t="s">
         <v>25</v>
       </c>
       <c r="AJ5" s="20"/>
-      <c r="AK5" s="34">
+      <c r="AK5" s="25">
         <v>50</v>
       </c>
-      <c r="AM5" s="27"/>
+      <c r="AM5" s="39"/>
       <c r="AN5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="AO5" s="20"/>
-      <c r="AP5" s="34">
+      <c r="AP5" s="25">
         <v>100</v>
       </c>
       <c r="AR5" s="14" t="s">
@@ -1507,12 +1507,12 @@
         <f>LigaEliminatória!C29</f>
         <v>0</v>
       </c>
-      <c r="AY5" s="27"/>
+      <c r="AY5" s="39"/>
       <c r="AZ5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="BA5" s="20"/>
-      <c r="BB5" s="34">
+      <c r="BB5" s="25">
         <v>200</v>
       </c>
     </row>
@@ -1528,7 +1528,7 @@
         <f>LigaPrincipal!G5</f>
         <v>0</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="26">
         <v>50</v>
       </c>
       <c r="G6" s="15" t="s">
@@ -1542,7 +1542,7 @@
         <f>LigaPrincipal!G11</f>
         <v>0</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="26">
         <v>50</v>
       </c>
       <c r="L6" s="15" t="s">
@@ -1556,7 +1556,7 @@
         <f>LigaPrincipal!G17</f>
         <v>0</v>
       </c>
-      <c r="O6" s="35">
+      <c r="O6" s="26">
         <v>50</v>
       </c>
       <c r="Q6" s="15" t="s">
@@ -1574,7 +1574,7 @@
         <f>LigaPrincipal!H23</f>
         <v>0</v>
       </c>
-      <c r="U6" s="35">
+      <c r="U6" s="26">
         <v>50</v>
       </c>
       <c r="W6" s="14" t="s">
@@ -1588,10 +1588,10 @@
         <f>LigaPrincipal!C5</f>
         <v>2</v>
       </c>
-      <c r="Z6" s="34">
+      <c r="Z6" s="25">
         <v>600</v>
       </c>
-      <c r="AB6" s="24" t="s">
+      <c r="AB6" s="43" t="s">
         <v>30</v>
       </c>
       <c r="AC6" s="13" t="s">
@@ -1605,23 +1605,23 @@
         <f>LigaPrincipal!M5</f>
         <v>0</v>
       </c>
-      <c r="AF6" s="36">
+      <c r="AF6" s="27">
         <v>100</v>
       </c>
-      <c r="AH6" s="28"/>
+      <c r="AH6" s="40"/>
       <c r="AI6" s="15" t="s">
         <v>26</v>
       </c>
       <c r="AJ6" s="21"/>
-      <c r="AK6" s="35">
+      <c r="AK6" s="26">
         <v>30</v>
       </c>
-      <c r="AM6" s="28"/>
+      <c r="AM6" s="40"/>
       <c r="AN6" s="15" t="s">
         <v>11</v>
       </c>
       <c r="AO6" s="21"/>
-      <c r="AP6" s="35">
+      <c r="AP6" s="26">
         <v>50</v>
       </c>
       <c r="AR6" s="14" t="s">
@@ -1646,12 +1646,12 @@
         <f>LigaEliminatória!C30</f>
         <v>0</v>
       </c>
-      <c r="AY6" s="28"/>
+      <c r="AY6" s="40"/>
       <c r="AZ6" s="15" t="s">
         <v>11</v>
       </c>
       <c r="BA6" s="21"/>
-      <c r="BB6" s="35">
+      <c r="BB6" s="26">
         <v>100</v>
       </c>
     </row>
@@ -1667,10 +1667,10 @@
         <f>LigaPrincipal!C6</f>
         <v>3</v>
       </c>
-      <c r="Z7" s="34">
+      <c r="Z7" s="25">
         <v>500</v>
       </c>
-      <c r="AB7" s="25"/>
+      <c r="AB7" s="44"/>
       <c r="AC7" s="15" t="s">
         <v>10</v>
       </c>
@@ -1682,27 +1682,27 @@
         <f>LigaPrincipal!M6</f>
         <v>0</v>
       </c>
-      <c r="AF7" s="35">
+      <c r="AF7" s="26">
         <v>50</v>
       </c>
-      <c r="AH7" s="26">
+      <c r="AH7" s="38">
         <v>2</v>
       </c>
       <c r="AI7" s="13" t="s">
         <v>24</v>
       </c>
       <c r="AJ7" s="19"/>
-      <c r="AK7" s="36">
+      <c r="AK7" s="27">
         <v>150</v>
       </c>
-      <c r="AM7" s="26">
+      <c r="AM7" s="38">
         <v>2</v>
       </c>
       <c r="AN7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="AO7" s="19"/>
-      <c r="AP7" s="36">
+      <c r="AP7" s="27">
         <v>150</v>
       </c>
       <c r="AR7" s="14" t="s">
@@ -1727,22 +1727,22 @@
         <f>LigaEliminatória!C31</f>
         <v>0</v>
       </c>
-      <c r="AY7" s="26">
+      <c r="AY7" s="38">
         <v>2</v>
       </c>
       <c r="AZ7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="BA7" s="19"/>
-      <c r="BB7" s="36">
+      <c r="BB7" s="27">
         <v>300</v>
       </c>
     </row>
     <row r="8" spans="2:54" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="17"/>
       <c r="W8" s="14" t="s">
         <v>16</v>
@@ -1755,10 +1755,10 @@
         <f>LigaPrincipal!C7</f>
         <v>4</v>
       </c>
-      <c r="Z8" s="34">
+      <c r="Z8" s="25">
         <v>400</v>
       </c>
-      <c r="AB8" s="24" t="s">
+      <c r="AB8" s="43" t="s">
         <v>31</v>
       </c>
       <c r="AC8" s="13" t="s">
@@ -1772,23 +1772,23 @@
         <f>LigaPrincipal!M7</f>
         <v>0</v>
       </c>
-      <c r="AF8" s="36">
+      <c r="AF8" s="27">
         <v>100</v>
       </c>
-      <c r="AH8" s="27"/>
+      <c r="AH8" s="39"/>
       <c r="AI8" s="14" t="s">
         <v>25</v>
       </c>
       <c r="AJ8" s="20"/>
-      <c r="AK8" s="34">
+      <c r="AK8" s="25">
         <v>50</v>
       </c>
-      <c r="AM8" s="27"/>
+      <c r="AM8" s="39"/>
       <c r="AN8" s="14" t="s">
         <v>10</v>
       </c>
       <c r="AO8" s="20"/>
-      <c r="AP8" s="34">
+      <c r="AP8" s="25">
         <v>100</v>
       </c>
       <c r="AR8" s="14" t="s">
@@ -1813,12 +1813,12 @@
         <f>LigaEliminatória!C32</f>
         <v>0</v>
       </c>
-      <c r="AY8" s="27"/>
+      <c r="AY8" s="39"/>
       <c r="AZ8" s="14" t="s">
         <v>10</v>
       </c>
       <c r="BA8" s="20"/>
-      <c r="BB8" s="34">
+      <c r="BB8" s="25">
         <v>200</v>
       </c>
     </row>
@@ -1839,10 +1839,10 @@
         <f>LigaPrincipal!C8</f>
         <v>5</v>
       </c>
-      <c r="Z9" s="34">
+      <c r="Z9" s="25">
         <v>350</v>
       </c>
-      <c r="AB9" s="25"/>
+      <c r="AB9" s="44"/>
       <c r="AC9" s="15" t="s">
         <v>10</v>
       </c>
@@ -1854,23 +1854,23 @@
         <f>LigaPrincipal!M8</f>
         <v>0</v>
       </c>
-      <c r="AF9" s="35">
+      <c r="AF9" s="26">
         <v>50</v>
       </c>
-      <c r="AH9" s="28"/>
+      <c r="AH9" s="40"/>
       <c r="AI9" s="15" t="s">
         <v>26</v>
       </c>
       <c r="AJ9" s="21"/>
-      <c r="AK9" s="35">
+      <c r="AK9" s="26">
         <v>30</v>
       </c>
-      <c r="AM9" s="28"/>
+      <c r="AM9" s="40"/>
       <c r="AN9" s="15" t="s">
         <v>11</v>
       </c>
       <c r="AO9" s="21"/>
-      <c r="AP9" s="35">
+      <c r="AP9" s="26">
         <v>50</v>
       </c>
       <c r="AR9" s="14" t="s">
@@ -1895,12 +1895,12 @@
         <f>LigaEliminatória!C33</f>
         <v>0</v>
       </c>
-      <c r="AY9" s="28"/>
+      <c r="AY9" s="40"/>
       <c r="AZ9" s="15" t="s">
         <v>11</v>
       </c>
       <c r="BA9" s="21"/>
-      <c r="BB9" s="35">
+      <c r="BB9" s="26">
         <v>100</v>
       </c>
     </row>
@@ -1921,10 +1921,10 @@
         <f>LigaPrincipal!C9</f>
         <v>6</v>
       </c>
-      <c r="Z10" s="34">
+      <c r="Z10" s="25">
         <v>300</v>
       </c>
-      <c r="AB10" s="24" t="s">
+      <c r="AB10" s="43" t="s">
         <v>32</v>
       </c>
       <c r="AC10" s="13" t="s">
@@ -1938,27 +1938,27 @@
         <f>LigaPrincipal!M9</f>
         <v>0</v>
       </c>
-      <c r="AF10" s="36">
+      <c r="AF10" s="27">
         <v>100</v>
       </c>
-      <c r="AH10" s="26">
+      <c r="AH10" s="38">
         <v>3</v>
       </c>
       <c r="AI10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="AJ10" s="19"/>
-      <c r="AK10" s="36">
+      <c r="AK10" s="27">
         <v>150</v>
       </c>
-      <c r="AM10" s="26">
+      <c r="AM10" s="38">
         <v>3</v>
       </c>
       <c r="AN10" s="13" t="s">
         <v>9</v>
       </c>
       <c r="AO10" s="19"/>
-      <c r="AP10" s="36">
+      <c r="AP10" s="27">
         <v>150</v>
       </c>
       <c r="AR10" s="14" t="s">
@@ -1983,14 +1983,14 @@
         <f>LigaEliminatória!C34</f>
         <v>0</v>
       </c>
-      <c r="AY10" s="26">
+      <c r="AY10" s="38">
         <v>3</v>
       </c>
       <c r="AZ10" s="13" t="s">
         <v>9</v>
       </c>
       <c r="BA10" s="19"/>
-      <c r="BB10" s="36">
+      <c r="BB10" s="27">
         <v>300</v>
       </c>
     </row>
@@ -2011,10 +2011,10 @@
         <f>LigaPrincipal!C10</f>
         <v>7</v>
       </c>
-      <c r="Z11" s="34">
+      <c r="Z11" s="25">
         <v>250</v>
       </c>
-      <c r="AB11" s="25"/>
+      <c r="AB11" s="44"/>
       <c r="AC11" s="15" t="s">
         <v>10</v>
       </c>
@@ -2026,23 +2026,23 @@
         <f>LigaPrincipal!M10</f>
         <v>0</v>
       </c>
-      <c r="AF11" s="35">
+      <c r="AF11" s="26">
         <v>50</v>
       </c>
-      <c r="AH11" s="27"/>
+      <c r="AH11" s="39"/>
       <c r="AI11" s="14" t="s">
         <v>25</v>
       </c>
       <c r="AJ11" s="20"/>
-      <c r="AK11" s="34">
+      <c r="AK11" s="25">
         <v>50</v>
       </c>
-      <c r="AM11" s="27"/>
+      <c r="AM11" s="39"/>
       <c r="AN11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="AO11" s="20"/>
-      <c r="AP11" s="34">
+      <c r="AP11" s="25">
         <v>100</v>
       </c>
       <c r="AR11" s="14" t="s">
@@ -2067,12 +2067,12 @@
         <f>LigaEliminatória!C35</f>
         <v>0</v>
       </c>
-      <c r="AY11" s="27"/>
+      <c r="AY11" s="39"/>
       <c r="AZ11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="BA11" s="20"/>
-      <c r="BB11" s="34">
+      <c r="BB11" s="25">
         <v>200</v>
       </c>
     </row>
@@ -2093,10 +2093,10 @@
         <f>LigaPrincipal!C11</f>
         <v>8</v>
       </c>
-      <c r="Z12" s="34">
+      <c r="Z12" s="25">
         <v>200</v>
       </c>
-      <c r="AB12" s="24" t="s">
+      <c r="AB12" s="43" t="s">
         <v>33</v>
       </c>
       <c r="AC12" s="13" t="s">
@@ -2110,23 +2110,23 @@
         <f>LigaPrincipal!M11</f>
         <v>0</v>
       </c>
-      <c r="AF12" s="36">
+      <c r="AF12" s="27">
         <v>100</v>
       </c>
-      <c r="AH12" s="28"/>
+      <c r="AH12" s="40"/>
       <c r="AI12" s="15" t="s">
         <v>26</v>
       </c>
       <c r="AJ12" s="21"/>
-      <c r="AK12" s="35">
+      <c r="AK12" s="26">
         <v>30</v>
       </c>
-      <c r="AM12" s="28"/>
+      <c r="AM12" s="40"/>
       <c r="AN12" s="15" t="s">
         <v>11</v>
       </c>
       <c r="AO12" s="21"/>
-      <c r="AP12" s="35">
+      <c r="AP12" s="26">
         <v>50</v>
       </c>
       <c r="AR12" s="14" t="s">
@@ -2151,12 +2151,12 @@
         <f>LigaEliminatória!C36</f>
         <v>0</v>
       </c>
-      <c r="AY12" s="28"/>
+      <c r="AY12" s="40"/>
       <c r="AZ12" s="15" t="s">
         <v>11</v>
       </c>
       <c r="BA12" s="21"/>
-      <c r="BB12" s="35">
+      <c r="BB12" s="26">
         <v>100</v>
       </c>
     </row>
@@ -2177,10 +2177,10 @@
         <f>LigaPrincipal!C12</f>
         <v>9</v>
       </c>
-      <c r="Z13" s="35">
+      <c r="Z13" s="26">
         <v>150</v>
       </c>
-      <c r="AB13" s="25"/>
+      <c r="AB13" s="44"/>
       <c r="AC13" s="15" t="s">
         <v>10</v>
       </c>
@@ -2192,27 +2192,27 @@
         <f>LigaPrincipal!M12</f>
         <v>0</v>
       </c>
-      <c r="AF13" s="35">
+      <c r="AF13" s="26">
         <v>50</v>
       </c>
-      <c r="AH13" s="26">
+      <c r="AH13" s="38">
         <v>4</v>
       </c>
       <c r="AI13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="AJ13" s="19"/>
-      <c r="AK13" s="36">
+      <c r="AK13" s="27">
         <v>150</v>
       </c>
-      <c r="AM13" s="26">
+      <c r="AM13" s="38">
         <v>4</v>
       </c>
       <c r="AN13" s="13" t="s">
         <v>9</v>
       </c>
       <c r="AO13" s="19"/>
-      <c r="AP13" s="36">
+      <c r="AP13" s="27">
         <v>150</v>
       </c>
       <c r="AR13" s="14" t="s">
@@ -2237,24 +2237,24 @@
         <f>LigaEliminatória!C37</f>
         <v>0</v>
       </c>
-      <c r="AY13" s="26">
+      <c r="AY13" s="38">
         <v>4</v>
       </c>
       <c r="AZ13" s="13" t="s">
         <v>9</v>
       </c>
       <c r="BA13" s="19"/>
-      <c r="BB13" s="36">
+      <c r="BB13" s="27">
         <v>300</v>
       </c>
     </row>
     <row r="14" spans="2:54" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
       <c r="F14" s="17"/>
-      <c r="AB14" s="24" t="s">
+      <c r="AB14" s="43" t="s">
         <v>34</v>
       </c>
       <c r="AC14" s="13" t="s">
@@ -2268,23 +2268,23 @@
         <f>LigaPrincipal!M13</f>
         <v>0</v>
       </c>
-      <c r="AF14" s="36">
+      <c r="AF14" s="27">
         <v>100</v>
       </c>
-      <c r="AH14" s="27"/>
+      <c r="AH14" s="39"/>
       <c r="AI14" s="14" t="s">
         <v>25</v>
       </c>
       <c r="AJ14" s="20"/>
-      <c r="AK14" s="34">
+      <c r="AK14" s="25">
         <v>50</v>
       </c>
-      <c r="AM14" s="27"/>
+      <c r="AM14" s="39"/>
       <c r="AN14" s="14" t="s">
         <v>10</v>
       </c>
       <c r="AO14" s="20"/>
-      <c r="AP14" s="34">
+      <c r="AP14" s="25">
         <v>100</v>
       </c>
       <c r="AR14" s="14" t="s">
@@ -2309,12 +2309,12 @@
         <f>LigaEliminatória!C38</f>
         <v>0</v>
       </c>
-      <c r="AY14" s="27"/>
+      <c r="AY14" s="39"/>
       <c r="AZ14" s="14" t="s">
         <v>10</v>
       </c>
       <c r="BA14" s="20"/>
-      <c r="BB14" s="34">
+      <c r="BB14" s="25">
         <v>200</v>
       </c>
     </row>
@@ -2324,7 +2324,7 @@
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="AB15" s="25"/>
+      <c r="AB15" s="44"/>
       <c r="AC15" s="15" t="s">
         <v>10</v>
       </c>
@@ -2336,23 +2336,23 @@
         <f>LigaPrincipal!M14</f>
         <v>0</v>
       </c>
-      <c r="AF15" s="35">
+      <c r="AF15" s="26">
         <v>50</v>
       </c>
-      <c r="AH15" s="28"/>
+      <c r="AH15" s="40"/>
       <c r="AI15" s="15" t="s">
         <v>26</v>
       </c>
       <c r="AJ15" s="21"/>
-      <c r="AK15" s="35">
+      <c r="AK15" s="26">
         <v>30</v>
       </c>
-      <c r="AM15" s="28"/>
+      <c r="AM15" s="40"/>
       <c r="AN15" s="15" t="s">
         <v>11</v>
       </c>
       <c r="AO15" s="21"/>
-      <c r="AP15" s="35">
+      <c r="AP15" s="26">
         <v>50</v>
       </c>
       <c r="AR15" s="14" t="s">
@@ -2377,12 +2377,12 @@
         <f>LigaEliminatória!C39</f>
         <v>0</v>
       </c>
-      <c r="AY15" s="28"/>
+      <c r="AY15" s="40"/>
       <c r="AZ15" s="15" t="s">
         <v>11</v>
       </c>
       <c r="BA15" s="21"/>
-      <c r="BB15" s="35">
+      <c r="BB15" s="26">
         <v>100</v>
       </c>
     </row>
@@ -2392,7 +2392,7 @@
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="AB16" s="24" t="s">
+      <c r="AB16" s="43" t="s">
         <v>35</v>
       </c>
       <c r="AC16" s="13" t="s">
@@ -2406,27 +2406,27 @@
         <f>LigaPrincipal!M15</f>
         <v>0</v>
       </c>
-      <c r="AF16" s="36">
+      <c r="AF16" s="27">
         <v>100</v>
       </c>
-      <c r="AH16" s="26">
+      <c r="AH16" s="38">
         <v>5</v>
       </c>
       <c r="AI16" s="13" t="s">
         <v>24</v>
       </c>
       <c r="AJ16" s="19"/>
-      <c r="AK16" s="36">
+      <c r="AK16" s="27">
         <v>150</v>
       </c>
-      <c r="AM16" s="26">
+      <c r="AM16" s="38">
         <v>5</v>
       </c>
       <c r="AN16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="AO16" s="19"/>
-      <c r="AP16" s="36">
+      <c r="AP16" s="27">
         <v>150</v>
       </c>
       <c r="AR16" s="14" t="s">
@@ -2451,14 +2451,14 @@
         <f>LigaEliminatória!C40</f>
         <v>0</v>
       </c>
-      <c r="AY16" s="26">
+      <c r="AY16" s="38">
         <v>5</v>
       </c>
       <c r="AZ16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="BA16" s="19"/>
-      <c r="BB16" s="36">
+      <c r="BB16" s="27">
         <v>300</v>
       </c>
     </row>
@@ -2468,7 +2468,7 @@
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
-      <c r="AB17" s="25"/>
+      <c r="AB17" s="44"/>
       <c r="AC17" s="15" t="s">
         <v>10</v>
       </c>
@@ -2480,23 +2480,23 @@
         <f>LigaPrincipal!M16</f>
         <v>0</v>
       </c>
-      <c r="AF17" s="35">
+      <c r="AF17" s="26">
         <v>50</v>
       </c>
-      <c r="AH17" s="27"/>
+      <c r="AH17" s="39"/>
       <c r="AI17" s="14" t="s">
         <v>25</v>
       </c>
       <c r="AJ17" s="20"/>
-      <c r="AK17" s="34">
+      <c r="AK17" s="25">
         <v>50</v>
       </c>
-      <c r="AM17" s="27"/>
+      <c r="AM17" s="39"/>
       <c r="AN17" s="14" t="s">
         <v>10</v>
       </c>
       <c r="AO17" s="20"/>
-      <c r="AP17" s="34">
+      <c r="AP17" s="25">
         <v>100</v>
       </c>
       <c r="AR17" s="14" t="s">
@@ -2521,12 +2521,12 @@
         <f>LigaEliminatória!C41</f>
         <v>0</v>
       </c>
-      <c r="AY17" s="27"/>
+      <c r="AY17" s="39"/>
       <c r="AZ17" s="14" t="s">
         <v>10</v>
       </c>
       <c r="BA17" s="20"/>
-      <c r="BB17" s="34">
+      <c r="BB17" s="25">
         <v>200</v>
       </c>
     </row>
@@ -2536,7 +2536,7 @@
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
-      <c r="AB18" s="24" t="s">
+      <c r="AB18" s="43" t="s">
         <v>36</v>
       </c>
       <c r="AC18" s="13" t="s">
@@ -2550,23 +2550,23 @@
         <f>LigaPrincipal!M17</f>
         <v>0</v>
       </c>
-      <c r="AF18" s="36">
+      <c r="AF18" s="27">
         <v>100</v>
       </c>
-      <c r="AH18" s="28"/>
+      <c r="AH18" s="40"/>
       <c r="AI18" s="15" t="s">
         <v>26</v>
       </c>
       <c r="AJ18" s="21"/>
-      <c r="AK18" s="35">
+      <c r="AK18" s="26">
         <v>30</v>
       </c>
-      <c r="AM18" s="28"/>
+      <c r="AM18" s="40"/>
       <c r="AN18" s="15" t="s">
         <v>11</v>
       </c>
       <c r="AO18" s="21"/>
-      <c r="AP18" s="35">
+      <c r="AP18" s="26">
         <v>50</v>
       </c>
       <c r="AR18" s="14" t="s">
@@ -2591,12 +2591,12 @@
         <f>LigaEliminatória!C42</f>
         <v>0</v>
       </c>
-      <c r="AY18" s="28"/>
+      <c r="AY18" s="40"/>
       <c r="AZ18" s="15" t="s">
         <v>11</v>
       </c>
       <c r="BA18" s="21"/>
-      <c r="BB18" s="35">
+      <c r="BB18" s="26">
         <v>100</v>
       </c>
     </row>
@@ -2606,7 +2606,7 @@
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
-      <c r="AB19" s="25"/>
+      <c r="AB19" s="44"/>
       <c r="AC19" s="15" t="s">
         <v>10</v>
       </c>
@@ -2618,27 +2618,27 @@
         <f>LigaPrincipal!M18</f>
         <v>0</v>
       </c>
-      <c r="AF19" s="35">
+      <c r="AF19" s="26">
         <v>50</v>
       </c>
-      <c r="AH19" s="26">
+      <c r="AH19" s="38">
         <v>6</v>
       </c>
       <c r="AI19" s="13" t="s">
         <v>24</v>
       </c>
       <c r="AJ19" s="19"/>
-      <c r="AK19" s="36">
+      <c r="AK19" s="27">
         <v>150</v>
       </c>
-      <c r="AM19" s="26">
+      <c r="AM19" s="38">
         <v>6</v>
       </c>
       <c r="AN19" s="13" t="s">
         <v>9</v>
       </c>
       <c r="AO19" s="19"/>
-      <c r="AP19" s="36">
+      <c r="AP19" s="27">
         <v>150</v>
       </c>
       <c r="AR19" s="14" t="s">
@@ -2663,37 +2663,37 @@
         <f>LigaEliminatória!C43</f>
         <v>0</v>
       </c>
-      <c r="AY19" s="26">
+      <c r="AY19" s="38">
         <v>6</v>
       </c>
       <c r="AZ19" s="13" t="s">
         <v>9</v>
       </c>
       <c r="BA19" s="19"/>
-      <c r="BB19" s="36">
+      <c r="BB19" s="27">
         <v>300</v>
       </c>
     </row>
     <row r="20" spans="2:54" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="AH20" s="27"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="AH20" s="39"/>
       <c r="AI20" s="14" t="s">
         <v>25</v>
       </c>
       <c r="AJ20" s="20"/>
-      <c r="AK20" s="34">
+      <c r="AK20" s="25">
         <v>50</v>
       </c>
-      <c r="AM20" s="27"/>
+      <c r="AM20" s="39"/>
       <c r="AN20" s="14" t="s">
         <v>10</v>
       </c>
       <c r="AO20" s="20"/>
-      <c r="AP20" s="34">
+      <c r="AP20" s="25">
         <v>100</v>
       </c>
       <c r="AR20" s="14" t="s">
@@ -2718,12 +2718,12 @@
         <f>LigaEliminatória!C44</f>
         <v>0</v>
       </c>
-      <c r="AY20" s="27"/>
+      <c r="AY20" s="39"/>
       <c r="AZ20" s="14" t="s">
         <v>10</v>
       </c>
       <c r="BA20" s="20"/>
-      <c r="BB20" s="34">
+      <c r="BB20" s="25">
         <v>200</v>
       </c>
     </row>
@@ -2733,20 +2733,20 @@
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
-      <c r="AH21" s="28"/>
+      <c r="AH21" s="40"/>
       <c r="AI21" s="15" t="s">
         <v>26</v>
       </c>
       <c r="AJ21" s="21"/>
-      <c r="AK21" s="35">
+      <c r="AK21" s="26">
         <v>30</v>
       </c>
-      <c r="AM21" s="28"/>
+      <c r="AM21" s="40"/>
       <c r="AN21" s="15" t="s">
         <v>11</v>
       </c>
       <c r="AO21" s="21"/>
-      <c r="AP21" s="35">
+      <c r="AP21" s="26">
         <v>50</v>
       </c>
       <c r="AR21" s="14" t="s">
@@ -2771,12 +2771,12 @@
         <f>LigaEliminatória!C45</f>
         <v>0</v>
       </c>
-      <c r="AY21" s="28"/>
+      <c r="AY21" s="40"/>
       <c r="AZ21" s="15" t="s">
         <v>11</v>
       </c>
       <c r="BA21" s="21"/>
-      <c r="BB21" s="35">
+      <c r="BB21" s="26">
         <v>100</v>
       </c>
     </row>
@@ -2786,24 +2786,24 @@
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
-      <c r="AH22" s="26">
+      <c r="AH22" s="38">
         <v>7</v>
       </c>
       <c r="AI22" s="13" t="s">
         <v>24</v>
       </c>
       <c r="AJ22" s="19"/>
-      <c r="AK22" s="36">
+      <c r="AK22" s="27">
         <v>150</v>
       </c>
-      <c r="AM22" s="26">
+      <c r="AM22" s="38">
         <v>7</v>
       </c>
       <c r="AN22" s="13" t="s">
         <v>9</v>
       </c>
       <c r="AO22" s="19"/>
-      <c r="AP22" s="36">
+      <c r="AP22" s="27">
         <v>150</v>
       </c>
       <c r="AR22" s="14" t="s">
@@ -2828,14 +2828,14 @@
         <f>LigaEliminatória!C46</f>
         <v>0</v>
       </c>
-      <c r="AY22" s="26">
+      <c r="AY22" s="38">
         <v>7</v>
       </c>
       <c r="AZ22" s="13" t="s">
         <v>9</v>
       </c>
       <c r="BA22" s="19"/>
-      <c r="BB22" s="36">
+      <c r="BB22" s="27">
         <v>300</v>
       </c>
     </row>
@@ -2845,20 +2845,20 @@
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
-      <c r="AH23" s="27"/>
+      <c r="AH23" s="39"/>
       <c r="AI23" s="14" t="s">
         <v>25</v>
       </c>
       <c r="AJ23" s="20"/>
-      <c r="AK23" s="34">
+      <c r="AK23" s="25">
         <v>50</v>
       </c>
-      <c r="AM23" s="27"/>
+      <c r="AM23" s="39"/>
       <c r="AN23" s="14" t="s">
         <v>10</v>
       </c>
       <c r="AO23" s="20"/>
-      <c r="AP23" s="34">
+      <c r="AP23" s="25">
         <v>100</v>
       </c>
       <c r="AR23" s="14" t="s">
@@ -2883,12 +2883,12 @@
         <f>LigaEliminatória!C47</f>
         <v>0</v>
       </c>
-      <c r="AY23" s="27"/>
+      <c r="AY23" s="39"/>
       <c r="AZ23" s="14" t="s">
         <v>10</v>
       </c>
       <c r="BA23" s="20"/>
-      <c r="BB23" s="34">
+      <c r="BB23" s="25">
         <v>200</v>
       </c>
     </row>
@@ -2898,20 +2898,20 @@
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
-      <c r="AH24" s="28"/>
+      <c r="AH24" s="40"/>
       <c r="AI24" s="15" t="s">
         <v>26</v>
       </c>
       <c r="AJ24" s="21"/>
-      <c r="AK24" s="35">
+      <c r="AK24" s="26">
         <v>30</v>
       </c>
-      <c r="AM24" s="28"/>
+      <c r="AM24" s="40"/>
       <c r="AN24" s="15" t="s">
         <v>11</v>
       </c>
       <c r="AO24" s="21"/>
-      <c r="AP24" s="35">
+      <c r="AP24" s="26">
         <v>50</v>
       </c>
       <c r="AR24" s="14" t="s">
@@ -2936,12 +2936,12 @@
         <f>LigaEliminatória!C48</f>
         <v>0</v>
       </c>
-      <c r="AY24" s="28"/>
+      <c r="AY24" s="40"/>
       <c r="AZ24" s="15" t="s">
         <v>11</v>
       </c>
       <c r="BA24" s="21"/>
-      <c r="BB24" s="35">
+      <c r="BB24" s="26">
         <v>100</v>
       </c>
     </row>
@@ -3042,22 +3042,22 @@
       </c>
     </row>
     <row r="30" spans="2:54" ht="28.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AR30" s="23" t="s">
+      <c r="AR30" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="AS30" s="23"/>
-      <c r="AT30" s="23"/>
-      <c r="AU30" s="23"/>
-      <c r="AV30" s="23"/>
-      <c r="AW30" s="23"/>
+      <c r="AS30" s="34"/>
+      <c r="AT30" s="34"/>
+      <c r="AU30" s="34"/>
+      <c r="AV30" s="34"/>
+      <c r="AW30" s="34"/>
     </row>
     <row r="31" spans="2:54" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AR31" s="4"/>
-      <c r="AS31" s="39" t="s">
+      <c r="AS31" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="AT31" s="40"/>
-      <c r="AU31" s="41"/>
+      <c r="AT31" s="32"/>
+      <c r="AU31" s="33"/>
       <c r="AV31" s="16" t="s">
         <v>13</v>
       </c>
@@ -3069,11 +3069,11 @@
       <c r="AR32" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="AS32" s="38"/>
-      <c r="AT32" s="38"/>
-      <c r="AU32" s="38"/>
+      <c r="AS32" s="37"/>
+      <c r="AT32" s="37"/>
+      <c r="AU32" s="37"/>
       <c r="AV32" s="19"/>
-      <c r="AW32" s="43">
+      <c r="AW32" s="28">
         <v>1000</v>
       </c>
     </row>
@@ -3081,11 +3081,11 @@
       <c r="AR33" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="AS33" s="37"/>
-      <c r="AT33" s="37"/>
-      <c r="AU33" s="37"/>
+      <c r="AS33" s="36"/>
+      <c r="AT33" s="36"/>
+      <c r="AU33" s="36"/>
       <c r="AV33" s="20"/>
-      <c r="AW33" s="44">
+      <c r="AW33" s="29">
         <v>500</v>
       </c>
     </row>
@@ -3093,11 +3093,11 @@
       <c r="AR34" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AS34" s="37"/>
-      <c r="AT34" s="37"/>
-      <c r="AU34" s="37"/>
+      <c r="AS34" s="36"/>
+      <c r="AT34" s="36"/>
+      <c r="AU34" s="36"/>
       <c r="AV34" s="20"/>
-      <c r="AW34" s="44">
+      <c r="AW34" s="29">
         <v>300</v>
       </c>
     </row>
@@ -3105,11 +3105,11 @@
       <c r="AR35" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AS35" s="37"/>
-      <c r="AT35" s="37"/>
-      <c r="AU35" s="37"/>
+      <c r="AS35" s="36"/>
+      <c r="AT35" s="36"/>
+      <c r="AU35" s="36"/>
       <c r="AV35" s="20"/>
-      <c r="AW35" s="44">
+      <c r="AW35" s="29">
         <v>250</v>
       </c>
     </row>
@@ -3117,49 +3117,34 @@
       <c r="AR36" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AS36" s="42"/>
-      <c r="AT36" s="42"/>
-      <c r="AU36" s="42"/>
+      <c r="AS36" s="35"/>
+      <c r="AT36" s="35"/>
+      <c r="AU36" s="35"/>
       <c r="AV36" s="21"/>
-      <c r="AW36" s="45">
+      <c r="AW36" s="30">
         <v>200</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="AS31:AU31"/>
-    <mergeCell ref="AR30:AW30"/>
-    <mergeCell ref="AS36:AU36"/>
-    <mergeCell ref="AS35:AU35"/>
-    <mergeCell ref="AS34:AU34"/>
-    <mergeCell ref="AS33:AU33"/>
-    <mergeCell ref="AS32:AU32"/>
-    <mergeCell ref="AY19:AY21"/>
-    <mergeCell ref="AY22:AY24"/>
-    <mergeCell ref="AH10:AH12"/>
-    <mergeCell ref="AH13:AH15"/>
-    <mergeCell ref="AH16:AH18"/>
-    <mergeCell ref="AY2:BB2"/>
-    <mergeCell ref="AY4:AY6"/>
-    <mergeCell ref="AY7:AY9"/>
-    <mergeCell ref="AY10:AY12"/>
-    <mergeCell ref="AY13:AY15"/>
-    <mergeCell ref="AY16:AY18"/>
-    <mergeCell ref="AM22:AM24"/>
+    <mergeCell ref="AR2:AW2"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="AB2:AF2"/>
+    <mergeCell ref="AB4:AB5"/>
+    <mergeCell ref="AB6:AB7"/>
+    <mergeCell ref="AH4:AH6"/>
+    <mergeCell ref="AH7:AH9"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AM4:AM6"/>
+    <mergeCell ref="AM7:AM9"/>
+    <mergeCell ref="AM10:AM12"/>
+    <mergeCell ref="AM13:AM15"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="AH19:AH21"/>
-    <mergeCell ref="AH22:AH24"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AM4:AM6"/>
-    <mergeCell ref="AM7:AM9"/>
-    <mergeCell ref="AM10:AM12"/>
-    <mergeCell ref="AM13:AM15"/>
-    <mergeCell ref="AM16:AM18"/>
-    <mergeCell ref="AM19:AM21"/>
     <mergeCell ref="W2:Z2"/>
     <mergeCell ref="AB10:AB11"/>
     <mergeCell ref="AB12:AB13"/>
@@ -3169,13 +3154,28 @@
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="AR2:AW2"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="AB2:AF2"/>
-    <mergeCell ref="AB4:AB5"/>
-    <mergeCell ref="AB6:AB7"/>
-    <mergeCell ref="AH4:AH6"/>
-    <mergeCell ref="AH7:AH9"/>
+    <mergeCell ref="AY2:BB2"/>
+    <mergeCell ref="AY4:AY6"/>
+    <mergeCell ref="AY7:AY9"/>
+    <mergeCell ref="AY10:AY12"/>
+    <mergeCell ref="AY13:AY15"/>
+    <mergeCell ref="AY19:AY21"/>
+    <mergeCell ref="AY22:AY24"/>
+    <mergeCell ref="AH10:AH12"/>
+    <mergeCell ref="AH13:AH15"/>
+    <mergeCell ref="AH16:AH18"/>
+    <mergeCell ref="AY16:AY18"/>
+    <mergeCell ref="AM22:AM24"/>
+    <mergeCell ref="AH22:AH24"/>
+    <mergeCell ref="AM16:AM18"/>
+    <mergeCell ref="AM19:AM21"/>
+    <mergeCell ref="AS31:AU31"/>
+    <mergeCell ref="AR30:AW30"/>
+    <mergeCell ref="AS36:AU36"/>
+    <mergeCell ref="AS35:AU35"/>
+    <mergeCell ref="AS34:AU34"/>
+    <mergeCell ref="AS33:AU33"/>
+    <mergeCell ref="AS32:AU32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3188,7 +3188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13D8C0E-9475-4AA4-AFE6-5C960D3D023D}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -3204,22 +3204,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="E1" s="31" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="E1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="J1" s="31" t="s">
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="J1" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -3260,7 +3260,7 @@
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="45" t="s">
         <v>29</v>
       </c>
       <c r="K3" s="1">
@@ -3280,7 +3280,7 @@
       <c r="E4" s="1">
         <v>2</v>
       </c>
-      <c r="J4" s="31"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1">
         <v>2</v>
       </c>
@@ -3298,7 +3298,7 @@
       <c r="E5" s="1">
         <v>3</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="45" t="s">
         <v>30</v>
       </c>
       <c r="K5" s="1">
@@ -3315,7 +3315,7 @@
       <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="J6" s="31"/>
+      <c r="J6" s="45"/>
       <c r="K6" s="1">
         <v>2</v>
       </c>
@@ -3330,12 +3330,12 @@
       <c r="C7" s="1">
         <v>4</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="J7" s="31" t="s">
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="J7" s="45" t="s">
         <v>31</v>
       </c>
       <c r="K7" s="1">
@@ -3358,7 +3358,7 @@
       <c r="G8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="31"/>
+      <c r="J8" s="45"/>
       <c r="K8" s="1">
         <v>2</v>
       </c>
@@ -3376,7 +3376,7 @@
       <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="J9" s="31" t="s">
+      <c r="J9" s="45" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="1">
@@ -3396,7 +3396,7 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="J10" s="31"/>
+      <c r="J10" s="45"/>
       <c r="K10" s="1">
         <v>2</v>
       </c>
@@ -3414,7 +3414,7 @@
       <c r="E11" s="1">
         <v>3</v>
       </c>
-      <c r="J11" s="31" t="s">
+      <c r="J11" s="45" t="s">
         <v>33</v>
       </c>
       <c r="K11" s="1">
@@ -3431,18 +3431,18 @@
       <c r="C12" s="1">
         <v>9</v>
       </c>
-      <c r="J12" s="31"/>
+      <c r="J12" s="45"/>
       <c r="K12" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="J13" s="31" t="s">
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="J13" s="45" t="s">
         <v>34</v>
       </c>
       <c r="K13" s="1">
@@ -3456,7 +3456,7 @@
       <c r="G14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="31"/>
+      <c r="J14" s="45"/>
       <c r="K14" s="1">
         <v>2</v>
       </c>
@@ -3465,7 +3465,7 @@
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="J15" s="31" t="s">
+      <c r="J15" s="45" t="s">
         <v>35</v>
       </c>
       <c r="K15" s="1">
@@ -3476,7 +3476,7 @@
       <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="J16" s="31"/>
+      <c r="J16" s="45"/>
       <c r="K16" s="1">
         <v>2</v>
       </c>
@@ -3485,7 +3485,7 @@
       <c r="E17" s="1">
         <v>3</v>
       </c>
-      <c r="J17" s="31" t="s">
+      <c r="J17" s="45" t="s">
         <v>36</v>
       </c>
       <c r="K17" s="1">
@@ -3493,18 +3493,18 @@
       </c>
     </row>
     <row r="18" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="J18" s="31"/>
+      <c r="J18" s="45"/>
       <c r="K18" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
     </row>
     <row r="20" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F20" s="1" t="s">
@@ -3534,11 +3534,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E19:H19"/>
     <mergeCell ref="J15:J16"/>
     <mergeCell ref="J17:J18"/>
     <mergeCell ref="J1:M1"/>
@@ -3548,6 +3543,11 @@
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="J13:J14"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E19:H19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>